<commit_message>
flu through step 1
</commit_message>
<xml_diff>
--- a/dependencies/virus/h7n3/script_dependents/Filtered_Regions.xlsx
+++ b/dependencies/virus/h7n3/script_dependents/Filtered_Regions.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tstuber/workspace/vSNP/dependencies/virus/h7n3/script_dependents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CF2981-97D9-524B-AE92-0D4F6FD1C734}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6719FE-9CA8-CE47-9DF3-B60C6607F9F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5220" yWindow="460" windowWidth="23580" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="H7N3-Seq1" sheetId="2" r:id="rId1"/>
-    <sheet name="H7N3-Seq2" sheetId="3" r:id="rId2"/>
-    <sheet name="H7N3-Seq3" sheetId="4" r:id="rId3"/>
-    <sheet name="H7N3-Seq4" sheetId="5" r:id="rId4"/>
-    <sheet name="H7N3-Seq5" sheetId="6" r:id="rId5"/>
-    <sheet name="H7N3-Seq6" sheetId="7" r:id="rId6"/>
-    <sheet name="H7N3-Seq7" sheetId="8" r:id="rId7"/>
-    <sheet name="H7N3-Seq8" sheetId="9" r:id="rId8"/>
+    <sheet name="H7N3Seq1" sheetId="2" r:id="rId1"/>
+    <sheet name="H7N3Seq2" sheetId="3" r:id="rId2"/>
+    <sheet name="H7N3Seq3" sheetId="4" r:id="rId3"/>
+    <sheet name="H7N3Seq4" sheetId="5" r:id="rId4"/>
+    <sheet name="H7N3Seq5" sheetId="6" r:id="rId5"/>
+    <sheet name="H7N3Seq6" sheetId="7" r:id="rId6"/>
+    <sheet name="H7N3Seq7" sheetId="8" r:id="rId7"/>
+    <sheet name="H7N3Seq8" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140001"/>
   <extLst>
@@ -2009,7 +2009,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E17584-1832-3947-8894-74B4FD35214B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>

<commit_message>
filter headers added, step 2 flu working
</commit_message>
<xml_diff>
--- a/dependencies/virus/h7n3/script_dependents/Filtered_Regions.xlsx
+++ b/dependencies/virus/h7n3/script_dependents/Filtered_Regions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tstuber/workspace/vSNP/dependencies/virus/h7n3/script_dependents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6719FE-9CA8-CE47-9DF3-B60C6607F9F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F657BE-F669-004B-8B9A-3597C60419C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5220" yWindow="460" windowWidth="23580" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,6 +29,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+  <si>
+    <t>H7N3-All</t>
+  </si>
+  <si>
+    <t>H7N3-01</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1913,11 +1927,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1925,8 +1939,23 @@
     <col min="1" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="14" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1" spans="1:2" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>